<commit_message>
continue benchmarking of px score. run os 1000x
</commit_message>
<xml_diff>
--- a/data/tableone_discovery_methylscoreaml_px.xlsx
+++ b/data/tableone_discovery_methylscoreaml_px.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="103">
-  <si>
-    <t>Grouped by MethylScore55_NewRiskEFS Categorical</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="106">
+  <si>
+    <t>Grouped by MethylScoreAML_Px Categorical</t>
   </si>
   <si>
     <t>Missing</t>
@@ -142,178 +142,187 @@
     <t>No</t>
   </si>
   <si>
-    <t>9.5 (6.4)</t>
-  </si>
-  <si>
-    <t>248 (48.4)</t>
-  </si>
-  <si>
-    <t>264 (51.6)</t>
-  </si>
-  <si>
-    <t>263 (51.4)</t>
-  </si>
-  <si>
-    <t>249 (48.6)</t>
-  </si>
-  <si>
-    <t>374 (78.9)</t>
-  </si>
-  <si>
-    <t>47 (9.9)</t>
-  </si>
-  <si>
-    <t>27 (5.7)</t>
-  </si>
-  <si>
-    <t>4 (0.8)</t>
-  </si>
-  <si>
-    <t>18 (3.8)</t>
-  </si>
-  <si>
-    <t>108 (21.6)</t>
-  </si>
-  <si>
-    <t>391 (78.4)</t>
-  </si>
-  <si>
-    <t>109 (23.9)</t>
-  </si>
-  <si>
-    <t>348 (76.1)</t>
-  </si>
-  <si>
-    <t>210 (41.0)</t>
-  </si>
-  <si>
-    <t>302 (59.0)</t>
-  </si>
-  <si>
-    <t>58.8 (24.8)</t>
-  </si>
-  <si>
-    <t>42 (8.3)</t>
-  </si>
-  <si>
-    <t>193 (38.2)</t>
-  </si>
-  <si>
-    <t>270 (53.5)</t>
-  </si>
-  <si>
-    <t>8 (1.6)</t>
-  </si>
-  <si>
-    <t>274 (53.5)</t>
-  </si>
-  <si>
-    <t>230 (44.9)</t>
-  </si>
-  <si>
-    <t>74 (14.5)</t>
-  </si>
-  <si>
-    <t>436 (85.5)</t>
-  </si>
-  <si>
-    <t>9.3 (6.3)</t>
-  </si>
-  <si>
-    <t>210 (49.1)</t>
-  </si>
-  <si>
-    <t>218 (50.9)</t>
-  </si>
-  <si>
-    <t>203 (47.4)</t>
-  </si>
-  <si>
-    <t>225 (52.6)</t>
-  </si>
-  <si>
-    <t>318 (79.1)</t>
-  </si>
-  <si>
-    <t>55 (13.7)</t>
-  </si>
-  <si>
-    <t>16 (4.0)</t>
-  </si>
-  <si>
-    <t>1 (0.2)</t>
-  </si>
-  <si>
-    <t>2 (0.5)</t>
-  </si>
-  <si>
-    <t>10 (2.5)</t>
-  </si>
-  <si>
-    <t>76 (18.4)</t>
-  </si>
-  <si>
-    <t>336 (81.6)</t>
-  </si>
-  <si>
-    <t>149 (40.9)</t>
-  </si>
-  <si>
-    <t>215 (59.1)</t>
-  </si>
-  <si>
-    <t>253 (59.1)</t>
-  </si>
-  <si>
-    <t>175 (40.9)</t>
-  </si>
-  <si>
-    <t>69.9 (22.7)</t>
-  </si>
-  <si>
-    <t>86 (20.4)</t>
-  </si>
-  <si>
-    <t>260 (61.8)</t>
-  </si>
-  <si>
-    <t>75 (17.8)</t>
-  </si>
-  <si>
-    <t>28 (6.5)</t>
-  </si>
-  <si>
-    <t>233 (54.4)</t>
-  </si>
-  <si>
-    <t>167 (39.0)</t>
-  </si>
-  <si>
-    <t>90 (21.0)</t>
-  </si>
-  <si>
-    <t>338 (79.0)</t>
-  </si>
-  <si>
-    <t>0.599</t>
-  </si>
-  <si>
-    <t>0.900</t>
-  </si>
-  <si>
-    <t>0.256</t>
-  </si>
-  <si>
-    <t>0.232</t>
-  </si>
-  <si>
-    <t>0.266</t>
+    <t>9.6 (6.2)</t>
+  </si>
+  <si>
+    <t>348 (49.2)</t>
+  </si>
+  <si>
+    <t>359 (50.8)</t>
+  </si>
+  <si>
+    <t>357 (50.5)</t>
+  </si>
+  <si>
+    <t>350 (49.5)</t>
+  </si>
+  <si>
+    <t>521 (79.1)</t>
+  </si>
+  <si>
+    <t>68 (10.3)</t>
+  </si>
+  <si>
+    <t>36 (5.5)</t>
+  </si>
+  <si>
+    <t>4 (0.6)</t>
+  </si>
+  <si>
+    <t>6 (0.9)</t>
+  </si>
+  <si>
+    <t>24 (3.6)</t>
+  </si>
+  <si>
+    <t>137 (19.9)</t>
+  </si>
+  <si>
+    <t>551 (80.1)</t>
+  </si>
+  <si>
+    <t>178 (28.5)</t>
+  </si>
+  <si>
+    <t>447 (71.5)</t>
+  </si>
+  <si>
+    <t>355 (50.2)</t>
+  </si>
+  <si>
+    <t>352 (49.8)</t>
+  </si>
+  <si>
+    <t>61.3 (24.8)</t>
+  </si>
+  <si>
+    <t>89 (12.8)</t>
+  </si>
+  <si>
+    <t>276 (39.7)</t>
+  </si>
+  <si>
+    <t>331 (47.6)</t>
+  </si>
+  <si>
+    <t>27 (3.8)</t>
+  </si>
+  <si>
+    <t>370 (52.3)</t>
+  </si>
+  <si>
+    <t>310 (43.8)</t>
+  </si>
+  <si>
+    <t>133 (18.8)</t>
+  </si>
+  <si>
+    <t>573 (81.2)</t>
+  </si>
+  <si>
+    <t>8.7 (6.6)</t>
+  </si>
+  <si>
+    <t>110 (47.2)</t>
+  </si>
+  <si>
+    <t>123 (52.8)</t>
+  </si>
+  <si>
+    <t>109 (46.8)</t>
+  </si>
+  <si>
+    <t>124 (53.2)</t>
+  </si>
+  <si>
+    <t>171 (78.8)</t>
+  </si>
+  <si>
+    <t>34 (15.7)</t>
+  </si>
+  <si>
+    <t>7 (3.2)</t>
+  </si>
+  <si>
+    <t>1 (0.5)</t>
+  </si>
+  <si>
+    <t>4 (1.8)</t>
+  </si>
+  <si>
+    <t>47 (21.1)</t>
+  </si>
+  <si>
+    <t>176 (78.9)</t>
+  </si>
+  <si>
+    <t>80 (40.8)</t>
+  </si>
+  <si>
+    <t>116 (59.2)</t>
+  </si>
+  <si>
+    <t>108 (46.4)</t>
+  </si>
+  <si>
+    <t>125 (53.6)</t>
+  </si>
+  <si>
+    <t>71.4 (22.2)</t>
+  </si>
+  <si>
+    <t>39 (17.0)</t>
+  </si>
+  <si>
+    <t>177 (77.0)</t>
+  </si>
+  <si>
+    <t>14 (6.1)</t>
+  </si>
+  <si>
+    <t>9 (3.9)</t>
+  </si>
+  <si>
+    <t>137 (58.8)</t>
+  </si>
+  <si>
+    <t>87 (37.3)</t>
+  </si>
+  <si>
+    <t>31 (13.4)</t>
+  </si>
+  <si>
+    <t>201 (86.6)</t>
+  </si>
+  <si>
+    <t>0.058</t>
+  </si>
+  <si>
+    <t>0.647</t>
+  </si>
+  <si>
+    <t>0.364</t>
+  </si>
+  <si>
+    <t>0.095</t>
+  </si>
+  <si>
+    <t>0.779</t>
+  </si>
+  <si>
+    <t>0.002</t>
+  </si>
+  <si>
+    <t>0.344</t>
   </si>
   <si>
     <t>&lt;0.001</t>
   </si>
   <si>
-    <t>0.011</t>
+    <t>0.211</t>
+  </si>
+  <si>
+    <t>0.071</t>
   </si>
   <si>
     <t>Two Sample T-test</t>
@@ -720,10 +729,10 @@
       </c>
       <c r="B4" s="1"/>
       <c r="D4">
-        <v>512</v>
+        <v>707</v>
       </c>
       <c r="E4">
-        <v>428</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -738,13 +747,13 @@
         <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F5" t="s">
         <v>93</v>
       </c>
       <c r="G5" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -761,13 +770,13 @@
         <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F6" t="s">
         <v>94</v>
       </c>
       <c r="G6" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -779,7 +788,7 @@
         <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -796,13 +805,13 @@
         <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F8" t="s">
         <v>95</v>
       </c>
       <c r="G8" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -814,7 +823,7 @@
         <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -831,13 +840,13 @@
         <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F10" t="s">
         <v>96</v>
       </c>
       <c r="G10" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -849,7 +858,7 @@
         <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -861,7 +870,7 @@
         <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -873,7 +882,7 @@
         <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -882,10 +891,7 @@
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -894,7 +900,7 @@
         <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E15" t="s">
         <v>77</v>
@@ -911,7 +917,7 @@
         <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s">
         <v>78</v>
@@ -920,7 +926,7 @@
         <v>97</v>
       </c>
       <c r="G16" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -929,7 +935,7 @@
         <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E17" t="s">
         <v>79</v>
@@ -946,7 +952,7 @@
         <v>119</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E18" t="s">
         <v>80</v>
@@ -955,7 +961,7 @@
         <v>98</v>
       </c>
       <c r="G18" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -964,7 +970,7 @@
         <v>31</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E19" t="s">
         <v>81</v>
@@ -981,16 +987,16 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E20" t="s">
         <v>82</v>
       </c>
       <c r="F20" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G20" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -999,7 +1005,7 @@
         <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E21" t="s">
         <v>83</v>
@@ -1014,16 +1020,16 @@
         <v>67</v>
       </c>
       <c r="D22" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E22" t="s">
         <v>84</v>
       </c>
       <c r="F22" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G22" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1037,16 +1043,16 @@
         <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E23" t="s">
         <v>85</v>
       </c>
       <c r="F23" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G23" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1055,7 +1061,7 @@
         <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E24" t="s">
         <v>86</v>
@@ -1067,7 +1073,7 @@
         <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E25" t="s">
         <v>87</v>
@@ -1084,16 +1090,16 @@
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E26" t="s">
         <v>88</v>
       </c>
       <c r="F26" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G26" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1102,7 +1108,7 @@
         <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E27" t="s">
         <v>89</v>
@@ -1114,7 +1120,7 @@
         <v>39</v>
       </c>
       <c r="D28" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E28" t="s">
         <v>90</v>
@@ -1131,16 +1137,16 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E29" t="s">
         <v>91</v>
       </c>
       <c r="F29" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="G29" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1149,7 +1155,7 @@
         <v>41</v>
       </c>
       <c r="D30" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E30" t="s">
         <v>92</v>

</xml_diff>